<commit_message>
Project Gantt Chart Ver. 2
Project Gantt Chart Ver. 2
-Derrick Ward
</commit_message>
<xml_diff>
--- a/Project Gant Chart.xlsx
+++ b/Project Gant Chart.xlsx
@@ -127,8 +127,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -139,11 +141,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -301,7 +305,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Duration</c:v>
+            <c:v>Duration (Days)</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -356,7 +360,7 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,7 +400,7 @@
         <c:axId val="2115155144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="41752.0"/>
+          <c:max val="41751.0"/>
           <c:min val="41653.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -409,7 +413,7 @@
         <c:crossAx val="2115165432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10.0"/>
+        <c:majorUnit val="7.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -443,8 +447,8 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -790,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -801,7 +805,7 @@
     <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -830,7 +834,7 @@
         <v>41675</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -846,7 +850,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -862,7 +866,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -876,8 +880,9 @@
       <c r="D5" s="1">
         <v>41681</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -892,7 +897,7 @@
         <v>41683</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -907,7 +912,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -922,7 +927,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -937,7 +942,7 @@
         <v>41692</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -952,7 +957,7 @@
         <v>41695</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -967,7 +972,7 @@
         <v>41700</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -982,7 +987,7 @@
         <v>41705</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1017,7 @@
         <v>41730</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>41736</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1051,10 +1056,10 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>41751</v>
+        <v>41745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project Gantt Chart Ver. 3
Project Gantt Chart Ver. 3
-Derrick Ward
</commit_message>
<xml_diff>
--- a/Project Gant Chart.xlsx
+++ b/Project Gant Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="0" windowWidth="21860" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="1700" yWindow="0" windowWidth="27100" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Tasks</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t>Buffer Week</t>
   </si>
 </sst>
 </file>
@@ -189,9 +192,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$17</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>SRS Document</c:v>
                 </c:pt>
@@ -239,16 +242,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Create and Installation Package for System Deployment</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Buffer Week</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$17</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>41654.0</c:v>
                 </c:pt>
@@ -296,6 +302,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>41742.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41745.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,12 +317,71 @@
             <c:v>Duration (Days)</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>SRS Document</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Coding Standard</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bug Tracking Policy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Design User Interfaces</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Develop User Manual</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Risk Assessment</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Architectural Design for CTC Office and Signaling</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Design each major Architectural Component, and Interfaces</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Quality Assurance Plan, Specific Test Plan, and Setup Build Environ.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Develop UML Designs for each Component</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Coordinate on Design Review Presentations</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Create Test Cases</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>System Implementation (Classes)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sub-System Integration</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Test the System</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Create and Installation Package for System Deployment</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Buffer Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$17</c:f>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>21.0</c:v>
                 </c:pt>
@@ -361,6 +429,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,11 +447,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2115165432"/>
-        <c:axId val="2115155144"/>
+        <c:axId val="2117258904"/>
+        <c:axId val="2096696072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115165432"/>
+        <c:axId val="2117258904"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -389,7 +460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115155144"/>
+        <c:crossAx val="2096696072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -397,7 +468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115155144"/>
+        <c:axId val="2096696072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41751.0"/>
@@ -410,7 +481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115165432"/>
+        <c:crossAx val="2117258904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.0"/>
@@ -442,15 +513,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -467,6 +538,99 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11696700" y="4521200"/>
+          <a:ext cx="1244600" cy="1727200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Due Dates:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Work</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Package 1: 02/14/14</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Work Package 2: 03/27/14</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Work Package 3: 04/24/2014</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -794,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -842,7 +1006,7 @@
         <v>41668</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" si="0">D3-B3</f>
+        <f t="shared" ref="C3:C18" si="0">D3-B3</f>
         <v>6</v>
       </c>
       <c r="D3" s="1">
@@ -1060,6 +1224,21 @@
       </c>
       <c r="D17" s="1">
         <v>41745</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41745</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D18" s="1">
+        <v>41752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>